<commit_message>
Refactorisation et optimisation du téléchargement des articles arxiv
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -458,6 +458,11 @@
           <t>Lien de l'article</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Fichier</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -470,13 +475,13 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dhruv Sarkar, Samrat Mukhopadhyay, Abhishek Sinha</t>
+          <t>Dhruv Sarkar</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-08-23</t>
+          <t>2025-08-23T11:21:24+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -489,7 +494,11 @@
           <t>http://arxiv.org/abs/2508.16992v1</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2508.16992v1.Online_Learning_for_Approximately_Convex_Functions_with_Long_term_Adversarial_Constraints.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -502,13 +511,13 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Anders Aamand, Justin Y. Chen, Siddharth Gollapudi, Sandeep Silwal, Hao Wu</t>
+          <t>Anders Aamand</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-29</t>
+          <t>2025-05-29T19:47:09+00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -521,7 +530,11 @@
           <t>http://arxiv.org/abs/2505.23967v1</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2505.23967v1.Improved_Approximations_for_Hard_Graph_Problems_using_Predictions.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -534,13 +547,13 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Simone Foderà, Gloria Turati, Riccardo Nembrini, Maurizio Ferrari Dacrema, Paolo Cremonesi</t>
+          <t>Simone Foderà</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2024-09-09</t>
+          <t>2024-09-09T10:07:12+00:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -553,7 +566,11 @@
           <t>http://arxiv.org/abs/2409.05475v1</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2409.05475v1.Reinforcement_Learning_for_Variational_Quantum_Circuits_Design.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -566,7 +583,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Yanhui Zhu, Samik Basu, A. Pavan</t>
+          <t>Yanhui Zhu</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -576,7 +593,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024-08-08</t>
+          <t>2024-08-08T17:50:16+00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -589,7 +606,11 @@
           <t>http://arxiv.org/abs/2408.04620v2</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2408.04620v2.Regularized_Unconstrained_Weakly_Submodular_Maximization.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -602,13 +623,13 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Yang Liu, Chuan Zhou, Peng Zhang, Shirui Pan, Zhao Li, Hongyang Chen</t>
+          <t>Yang Liu</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024-06-05</t>
+          <t>2024-06-05T22:52:27+00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -621,7 +642,11 @@
           <t>http://arxiv.org/abs/2406.03647v2</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2406.03647v2.Decision_focused_Graph_Neural_Networks_for_Combinatorial_Optimization.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -634,13 +659,13 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Morris Yau, Nikolaos Karalias, Eric Lu, Jessica Xu, Stefanie Jegelka</t>
+          <t>Morris Yau</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-10-01</t>
+          <t>2023-10-01T00:12:31+00:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -653,7 +678,11 @@
           <t>http://arxiv.org/abs/2310.00526v7</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2310.00526v7.Are_Graph_Neural_Networks_Optimal_Approximation_Algorithms_.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -666,13 +695,13 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Davin Choo, Kirankumar Shiragur</t>
+          <t>Davin Choo</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-01-09</t>
+          <t>2023-01-09T06:25:44+00:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -685,7 +714,11 @@
           <t>http://arxiv.org/abs/2301.03180v3</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2301.03180v3.Subset_verification_and_search_algorithms_for_causal_DAGs.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -704,7 +737,7 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2022-08-12</t>
+          <t>2022-08-12T21:27:20+00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -717,7 +750,11 @@
           <t>http://arxiv.org/abs/2208.06506v3</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2208.06506v3.Optimal_LP_Rounding_and_Linear_Time_Approximation_Algorithms_for_Clustering_Edge_Colored_Hypergraphs.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -730,13 +767,13 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>David Ireland, Giovanni Montana</t>
+          <t>David Ireland</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2022-05-20</t>
+          <t>2022-05-20T11:54:03+00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -749,7 +786,11 @@
           <t>http://arxiv.org/abs/2205.10106v1</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2205.10106v1.LeNSE__Learning_To_Navigate_Subgraph_Embeddings_for_Large_Scale_Combinatorial_Optimisation.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -762,13 +803,13 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Seth Poulsen, Shubhang Kulkarni, Geoffrey Herman, Matthew West</t>
+          <t>Seth Poulsen</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2022-04-08</t>
+          <t>2022-04-08T17:44:59+00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -781,7 +822,11 @@
           <t>http://arxiv.org/abs/2204.04196v3</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2204.04196v3.Efficient_Feedback_and_Partial_Credit_Grading_for_Proof_Blocks_Problems.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -794,13 +839,13 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Soheil Behnezhad, Avrim Blum, Mahsa Derakhshan</t>
+          <t>Soheil Behnezhad</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2021-12-10</t>
+          <t>2021-12-10T09:46:12+00:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -813,7 +858,11 @@
           <t>http://arxiv.org/abs/2112.05415v1</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2112.05415v1.Stochastic_Vertex_Cover_with_Few_Queries.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -826,7 +875,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Martin J. A. Schuetz, J. Kyle Brubaker, Helmut G. Katzgraber</t>
+          <t>Martin J. A. Schuetz</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -836,7 +885,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2021-07-02</t>
+          <t>2021-07-02T16:54:35+00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -849,7 +898,11 @@
           <t>http://arxiv.org/abs/2107.01188v2</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2107.01188v2.Combinatorial_Optimization_with_Physics_Inspired_Graph_Neural_Networks.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -862,13 +915,13 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Lukas Gianinazzi, Maximilian Fries, Nikoli Dryden, Tal Ben-Nun, Maciej Besta, Torsten Hoefler</t>
+          <t>Lukas Gianinazzi</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2021-06-07</t>
+          <t>2021-06-07T13:21:09+00:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -881,7 +934,11 @@
           <t>http://arxiv.org/abs/2106.03594v3</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2106.03594v3.Learning_Combinatorial_Node_Labeling_Algorithms.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -894,7 +951,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Magnús M. Halldórsson, Murilo S. de Lima</t>
+          <t>Magnús M. Halldórsson</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -904,7 +961,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2020-12-17</t>
+          <t>2020-12-17T09:54:24+00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -917,7 +974,11 @@
           <t>http://arxiv.org/abs/2012.09475v2</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2012.09475v2.Query_Competitive_Sorting_with_Uncertainty.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -930,13 +991,13 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Faisal N. Abu-Khzam, Mohamed Mahmoud Abd El-Wahab, Noureldin Yosri</t>
+          <t>Faisal N. Abu-Khzam</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2020-06-08</t>
+          <t>2020-06-08T15:40:04+00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -949,7 +1010,11 @@
           <t>http://arxiv.org/abs/2006.04689v1</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2006.04689v1.Graph_Minors_Meet_Machine_Learning__the_Power_of_Obstructions.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -962,13 +1027,13 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Yaoxin Li, Jing Liu, Guozheng Lin, Yueyuan Hou, Muyun Mou, Jiang Zhang</t>
+          <t>Yaoxin Li</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2020-04-14</t>
+          <t>2020-04-14T14:11:00+00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -981,7 +1046,11 @@
           <t>http://arxiv.org/abs/2004.07300v1</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2004.07300v1.Gumbel_softmax_based_Optimization__A_Simple_General_Framework_for_Optimization_Problems_on_Graphs.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -994,13 +1063,13 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Evripidis Bampis, Dimitris Christou, Bruno Escoffier, Nguyen Kim Thang</t>
+          <t>Evripidis Bampis</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2019-07-12</t>
+          <t>2019-07-12T20:37:07+00:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1013,7 +1082,11 @@
           <t>http://arxiv.org/abs/1907.05944v2</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1907.05944v2.Online_learning_for_min_max_discrete_problems.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1026,13 +1099,13 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ryoma Sato, Makoto Yamada, Hisashi Kashima</t>
+          <t>Ryoma Sato</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2019-05-24</t>
+          <t>2019-05-24T14:41:17+00:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1045,7 +1118,11 @@
           <t>http://arxiv.org/abs/1905.10261v2</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>1905.10261v2.Approximation_Ratios_of_Graph_Neural_Networks_for_Combinatorial_Problems.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1058,13 +1135,13 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ceyhun Eksin, Keith Paarporn</t>
+          <t>Ceyhun Eksin</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2018-12-08</t>
+          <t>2018-12-08T18:51:51+00:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1077,7 +1154,11 @@
           <t>http://arxiv.org/abs/1812.03366v2</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>1812.03366v2.Control_of_learning_in_anti_coordination_network_games.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1090,13 +1171,13 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Mohsen Ghaffari, Jara Uitto</t>
+          <t>Mohsen Ghaffari</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2018-07-17</t>
+          <t>2018-07-17T07:01:03+00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1109,7 +1190,11 @@
           <t>http://arxiv.org/abs/1807.06251v1</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>1807.06251v1.Sparsifying_Distributed_Algorithms_with_Ramifications_in_Massively_Parallel_Computation_and_Centralized_Local_Computation.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1122,13 +1207,13 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Daniel Selsam, Matthew Lamm, Benedikt Bünz, Percy Liang, Leonardo de Moura, David L. Dill</t>
+          <t>Daniel Selsam</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2018-02-11</t>
+          <t>2018-02-11T03:04:28+00:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1141,7 +1226,11 @@
           <t>http://arxiv.org/abs/1802.03685v4</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>1802.03685v4.Learning_a_SAT_Solver_from_Single_Bit_Supervision.pdf</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1154,13 +1243,13 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Hanjun Dai, Elias B. Khalil, Yuyu Zhang, Bistra Dilkina, Le Song</t>
+          <t>Hanjun Dai</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2017-04-05</t>
+          <t>2017-04-05T23:08:07+00:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1173,7 +1262,11 @@
           <t>http://arxiv.org/abs/1704.01665v4</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1704.01665v4.Learning_Combinatorial_Optimization_Algorithms_over_Graphs.pdf</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
extraction des informations des conjectures json dans le fichier excel.
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Articles" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Conjectures" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -420,7 +419,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -478,7 +477,6 @@
           <t>Dhruv Sarkar</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
           <t>2025-08-23T11:21:24+00:00</t>
@@ -514,7 +512,6 @@
           <t>Anders Aamand</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>2025-05-29T19:47:09+00:00</t>
@@ -550,7 +547,6 @@
           <t>Simone Foderà</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>2024-09-09T10:07:12+00:00</t>
@@ -626,7 +622,6 @@
           <t>Yang Liu</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>2024-06-05T22:52:27+00:00</t>
@@ -662,7 +657,6 @@
           <t>Morris Yau</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>2023-10-01T00:12:31+00:00</t>
@@ -698,7 +692,6 @@
           <t>Davin Choo</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>2023-01-09T06:25:44+00:00</t>
@@ -734,7 +727,6 @@
           <t>Nate Veldt</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>2022-08-12T21:27:20+00:00</t>
@@ -770,7 +762,6 @@
           <t>David Ireland</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>2022-05-20T11:54:03+00:00</t>
@@ -806,7 +797,6 @@
           <t>Seth Poulsen</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
           <t>2022-04-08T17:44:59+00:00</t>
@@ -842,7 +832,6 @@
           <t>Soheil Behnezhad</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>2021-12-10T09:46:12+00:00</t>
@@ -918,7 +907,6 @@
           <t>Lukas Gianinazzi</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
           <t>2021-06-07T13:21:09+00:00</t>
@@ -994,7 +982,6 @@
           <t>Faisal N. Abu-Khzam</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
           <t>2020-06-08T15:40:04+00:00</t>
@@ -1030,7 +1017,6 @@
           <t>Yaoxin Li</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
           <t>2020-04-14T14:11:00+00:00</t>
@@ -1066,7 +1052,6 @@
           <t>Evripidis Bampis</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
           <t>2019-07-12T20:37:07+00:00</t>
@@ -1102,7 +1087,6 @@
           <t>Ryoma Sato</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
           <t>2019-05-24T14:41:17+00:00</t>
@@ -1138,7 +1122,6 @@
           <t>Ceyhun Eksin</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
           <t>2018-12-08T18:51:51+00:00</t>
@@ -1174,7 +1157,6 @@
           <t>Mohsen Ghaffari</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
           <t>2018-07-17T07:01:03+00:00</t>
@@ -1210,7 +1192,6 @@
           <t>Daniel Selsam</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
           <t>2018-02-11T03:04:28+00:00</t>
@@ -1246,7 +1227,6 @@
           <t>Hanjun Dai</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
           <t>2017-04-05T23:08:07+00:00</t>
@@ -1279,13 +1259,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1303,6 +1283,250 @@
           <t>Page</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>"Is there an MIS LCA with query complexity poly(Δ log n) ?"</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>aucune conjecture</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ajout d'un pdf de test avec conjecture et formule mathematique
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Articles" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,13 +413,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="112.42578125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="31.5703125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="135.7109375" bestFit="1" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1245,6 +1250,46 @@
       <c r="H23" t="inlineStr">
         <is>
           <t>1704.01665v4.Learning_Combinatorial_Optimization_Algorithms_over_Graphs.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Sami</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>test_overleaf.pdf</t>
         </is>
       </c>
     </row>
@@ -1259,13 +1304,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="53.85546875" bestFit="1" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1527,6 +1576,17 @@
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>aucune conjecture (json manquant)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ajout des autres fichiers texte
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\Desktop\memoire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C6305C-4AB4-4E2D-BD53-BBB0C6FDF773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BB47A7-9FB0-47DE-86C5-6C097A9A3D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="134">
   <si>
     <t>Id</t>
   </si>
@@ -405,41 +405,57 @@
     <t>Conjecture</t>
   </si>
   <si>
-    <t>These results suggest that NeuroSAT searches for a certificate of satisfiability, and that it only guesses sat once it has found one.</t>
-  </si>
-  <si>
-    <t>This suggests that NeuroSAT has not simply found a way to approximate SP, but rather has synthesized a qualitatively different algorithm.</t>
-  </si>
-  <si>
-    <t>Upon inspection, it seems to do so by learning to recognize the unsat cores.</t>
-  </si>
-  <si>
-    <t>We believe that their network's success is an instance of the phenomenon we study in this paper, namely that MPNNs can synthesize local search algorithms for constraint satisfaction problems.</t>
-  </si>
-  <si>
-    <t>We believe that architectures descended from NeuroSAT will be able to learn very different mechanisms and heuristics depending on the data they are trained on and the details of their objective functions.</t>
-  </si>
-  <si>
-    <t>We are cautiously optimistic that a descendant of NeuroSAT will one day lead to improvements to the state-of-the-art.</t>
-  </si>
-  <si>
     <t>Conjecture_id</t>
   </si>
   <si>
     <t>Parametre</t>
+  </si>
+  <si>
+    <t>Generalizations and strengthenings of Ryser's conjecture</t>
+  </si>
+  <si>
+    <t>2009.07239v3.pdf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2009.07239</t>
+  </si>
+  <si>
+    <t>Louis DeBiasio</t>
+  </si>
+  <si>
+    <t>fichier de test, pas inclus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Inter"/>
     </font>
   </fonts>
   <fills count="2">
@@ -459,13 +475,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -766,13 +789,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="112.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -784,7 +807,7 @@
     <col min="9" max="9" width="135.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -839,7 +862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -865,7 +888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -891,7 +914,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -920,7 +943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -946,7 +969,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -972,7 +995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -998,7 +1021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1024,7 +1047,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1050,7 +1073,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1076,7 +1099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1102,7 +1125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1131,7 +1154,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1157,7 +1180,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1186,7 +1209,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1212,7 +1235,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1238,7 +1261,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1264,7 +1287,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1290,7 +1313,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1316,7 +1339,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1342,7 +1365,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1368,7 +1391,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1394,27 +1417,57 @@
         <v>124</v>
       </c>
     </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G24" r:id="rId1" xr:uid="{98879843-8D25-4023-89BD-BA4BA592BD25}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="187.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -1423,72 +1476,6 @@
       </c>
       <c r="C1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1502,18 +1489,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generation du fichier excel
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\Desktop\memoire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BB47A7-9FB0-47DE-86C5-6C097A9A3D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41FF15B-590C-482F-9847-333F1A0EC5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="195">
   <si>
     <t>Id</t>
   </si>
@@ -66,39 +66,42 @@
     <t>http://arxiv.org/abs/2508.16992v1</t>
   </si>
   <si>
+    <t>JSON introuvable</t>
+  </si>
+  <si>
+    <t>2508.16992v1.Online_Learning_for_Approximately_Convex_Functions_with_Long_term_Adversarial_Constraints.pdf</t>
+  </si>
+  <si>
+    <t>Improved Approximations for Hard Graph Problems using Predictions</t>
+  </si>
+  <si>
+    <t>Anders Aamand</t>
+  </si>
+  <si>
+    <t>2025-05-29T19:47:09+00:00</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2505.23967v1</t>
+  </si>
+  <si>
+    <t>2505.23967v1.Improved_Approximations_for_Hard_Graph_Problems_using_Predictions.pdf</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning for Variational Quantum Circuits Design</t>
+  </si>
+  <si>
+    <t>Simone Foderà</t>
+  </si>
+  <si>
+    <t>2024-09-09T10:07:12+00:00</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2409.05475v1</t>
+  </si>
+  <si>
     <t>Non</t>
   </si>
   <si>
-    <t>2508.16992v1.Online_Learning_for_Approximately_Convex_Functions_with_Long_term_Adversarial_Constraints.pdf</t>
-  </si>
-  <si>
-    <t>Improved Approximations for Hard Graph Problems using Predictions</t>
-  </si>
-  <si>
-    <t>Anders Aamand</t>
-  </si>
-  <si>
-    <t>2025-05-29T19:47:09+00:00</t>
-  </si>
-  <si>
-    <t>http://arxiv.org/abs/2505.23967v1</t>
-  </si>
-  <si>
-    <t>2505.23967v1.Improved_Approximations_for_Hard_Graph_Problems_using_Predictions.pdf</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning for Variational Quantum Circuits Design</t>
-  </si>
-  <si>
-    <t>Simone Foderà</t>
-  </si>
-  <si>
-    <t>2024-09-09T10:07:12+00:00</t>
-  </si>
-  <si>
-    <t>http://arxiv.org/abs/2409.05475v1</t>
-  </si>
-  <si>
     <t>2409.05475v1.Reinforcement_Learning_for_Variational_Quantum_Circuits_Design.pdf</t>
   </si>
   <si>
@@ -399,31 +402,211 @@
     <t>1704.01665v4.Learning_Combinatorial_Optimization_Algorithms_over_Graphs.pdf</t>
   </si>
   <si>
+    <t>Generalizations and strengthenings of Ryser's conjecture</t>
+  </si>
+  <si>
+    <t>Louis DeBiasio</t>
+  </si>
+  <si>
+    <t>fichier de test, pas inclus</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2009.07239</t>
+  </si>
+  <si>
+    <t>2009.07239v3.pdf</t>
+  </si>
+  <si>
     <t>Article_id</t>
   </si>
   <si>
     <t>Conjecture</t>
   </si>
   <si>
+    <t>These results suggest that NeuroSAT searches for a certificate of satisfiability, and that it only guesses sat once it has found one.</t>
+  </si>
+  <si>
+    <t>This suggests that NeuroSAT has not simply found a way to approximate SP, but rather has synthesized a qualitatively different algorithm.</t>
+  </si>
+  <si>
+    <t>Upon inspection, it seems to do so by learning to recognize the unsat cores.</t>
+  </si>
+  <si>
+    <t>We believe that their network's success is an instance of the phenomenon we study in this paper, namely that MPNNs can synthesize local search algorithms for constraint satisfaction problems.</t>
+  </si>
+  <si>
+    <t>We believe that architectures descended from NeuroSAT will be able to learn very different mechanisms and heuristics depending on the data they are trained on and the details of their objective functions.</t>
+  </si>
+  <si>
+    <t>We are cautiously optimistic that a descendant of NeuroSAT will one day lead to improvements to the state-of-the-art.</t>
+  </si>
+  <si>
+    <t>Conjecture 2.1. For all integers $r \geq 2$, all $S \subseteq[r]$, and all $r$-colorings of a complete graph $K$, there exists a monochromatic $(r-1)$-cover consisting entirely of subgraphs having a color in $S$ or consisting entirely of subgraphs having a color in $[r] \backslash S$.</t>
+  </si>
+  <si>
+    <t>Conjecture 2.2. For all integers $r \geq 2$ and all $K \in \mathcal{K}_{r}, \operatorname{tc}_{r-1}(K) \leq r-1$. In particular, this implies that for every $r$-coloring of a complete graph $K$ and every color $i \in[r]$, either there is a monochromatic $(r-1)$-cover consisting entirely of subgraphs of color $i$, or entirely of subgraphs which don't have color $i$.</t>
+  </si>
+  <si>
+    <t>Conjecture 2.3. For all integers $r \geq 3$ and all $K \in \mathcal{K}_{r-1}, \operatorname{tc}_{r-1}(K) \leq r-1$. In particular, this implies that for every $r$-coloring of a complete graph $K$ and every color $i \in[r]$, either there is a monochromatic $(r-2)$-cover consisting entirely of subgraphs of color $i$, or a monochromatic $(r-1)$-cover consisting entirely of subgraphs which don't have color $i$.</t>
+  </si>
+  <si>
+    <t>Conjecture 2.4. For all integers $r \geq 2$, in every $r$-coloring of a complete graph $K$ there exists a monochromatic $(r-1)$-cover such that the monochromatic subgraphs have at most $\lceil r / 2\rceil$ different colors.</t>
+  </si>
+  <si>
+    <t>Conjecture 2.8. For all $\alpha \geq 1$, there exists $d=d(\alpha)$ such that for all $r \geq 2$, if $G$ is a graph with $\alpha(G)=\alpha$, then in every $r$-coloring of $G$, there exists a monochromatic $(r-1) \alpha$-cover consisting of subgraphs of diameter at most $d$.</t>
+  </si>
+  <si>
+    <t>Conjecture 2.14. There exists $d$ such that for all $r \geq 2$, if $K \in \mathcal{K}_{2}$, then in every $r$-coloring of $K$, there exists a monochromatic $(2 r-2)$-cover consisting of subgraphs of diameter at most d.</t>
+  </si>
+  <si>
+    <t>Conjecture 2.19. For all $r \geq 3$, in every $r$-coloring of $K_{n}^{r}$, there exists a monochromatic tightly connected subgraph which covers $V(K)$.</t>
+  </si>
+  <si>
+    <t>Conjecture 4.3. For all $\alpha \geq 1$, there exists $\delta=\delta(\alpha)$ such that for all $r \geq 2$, if $G$ is a graph with $\alpha(G)=\alpha$, then $\mathrm{dc}_{r}^{\delta}(G) \leq(r-1) \alpha$.</t>
+  </si>
+  <si>
+    <t>Conjecture 4.17. Let $G$ be a 3-colored complete graph. There exists a monochromatic 2-cover consisting of subgraphs of diameter at most 3.</t>
+  </si>
+  <si>
+    <t>Conjecture 4.22. Suppose $G$ is a complete 4-partite graph with vertex set partitioned as $\left\{V_{1}, V_{2}, V_{3}, V_{4}\right\}$. If $\left[V_{i}, V_{j}\right]$ is colored with colors from $[5] \backslash\{i, j\}$ for all distinct $i, j \in[4]$, then $G$ can be covered with at most three monochromatic subgraphs of bounded diameter.</t>
+  </si>
+  <si>
     <t>Conjecture_id</t>
   </si>
   <si>
     <t>Parametre</t>
   </si>
   <si>
-    <t>Generalizations and strengthenings of Ryser's conjecture</t>
-  </si>
-  <si>
-    <t>2009.07239v3.pdf</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/2009.07239</t>
-  </si>
-  <si>
-    <t>Louis DeBiasio</t>
-  </si>
-  <si>
-    <t>fichier de test, pas inclus</t>
+    <t>23-Conjecture 2.1</t>
+  </si>
+  <si>
+    <t>{'name': '$r$', 'definition': '$r$ is an integer with $r \\geq 2$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$S$', 'definition': '$S \\subseteq [r]$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$[r]$', 'definition': '$[r]=\\{1,2,\\dots,r\\}$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$K$', 'definition': '$K$ is a complete graph.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'r-coloring', 'definition': 'An $r$-coloring of the edges of a graph $G$ is a function $c:E(G) \\to [r]$; equivalently, a partition of $E(G)$ into (possibly empty) sets $\\{E_{1},\\ldots,E_{r}\\}$.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'monochromatic cover', 'definition': 'In an $r$-colored graph $H$, a monochromatic cover is a set $\\mathcal{T}$ of monochromatic connected subgraphs with $V(H)=\\cup_{T \\in \\mathcal{T}} V(T)$.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'monochromatic $t$-cover', 'definition': 'A monochromatic cover of order at most $t$.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 2.2</t>
+  </si>
+  <si>
+    <t>{'name': '$K$', 'definition': '$K \\in \\mathcal{K}_{r}$ is a complete $r$-partite graph.'}</t>
+  </si>
+  <si>
+    <t>{'name': '\\mathcal{K}_{k}', 'definition': 'For $k \\geq 2$, $\\mathcal{K}_{k}$ is the family of all complete $k$-partite graphs.'}</t>
+  </si>
+  <si>
+    <t>{'name': '\\operatorname{tc}_{r}(H)', 'definition': 'The minimum integer $t$ such that in every $r$-coloring of the edges of $H$, there exists a monochromatic $t$-cover of $H$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$i$', 'definition': '$i \\in [r]$ is a color index.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 2.3</t>
+  </si>
+  <si>
+    <t>{'name': '$r$', 'definition': '$r$ is an integer with $r \\geq 3$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$K$', 'definition': '$K \\in \\mathcal{K}_{r-1}$ is a complete $(r-1)$-partite graph.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 2.4</t>
+  </si>
+  <si>
+    <t>{'name': '\\lceil r/2 \\rceil', 'definition': 'The ceiling of $r/2$.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 2.8</t>
+  </si>
+  <si>
+    <t>{'name': '$\\alpha$', 'definition': '$\\alpha \\geq 1$ is an integer parameter.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$d$', 'definition': '$d=d(\\alpha)$ is a diameter bound depending on $\\alpha$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$G$', 'definition': '$G$ is a graph with $\\alpha(G)=\\alpha$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '\\alpha(G)', 'definition': 'The size of a maximum independent set of vertices in $G$.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'diameter', 'definition': 'For vertices $u,v \\in V(G)$, $d(u,v)$ is the length of the shortest $u,v$-path (or $\\infty$ if none exists); $\\operatorname{diam}(G)$ is the smallest $d$ with $d(u,v) \\le d$ for all $u,v \\in V(G)$.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 2.14</t>
+  </si>
+  <si>
+    <t>{'name': '$d$', 'definition': 'An absolute diameter bound.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$K$', 'definition': '$K \\in \\mathcal{K}_{2}$ is a complete bipartite graph.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 2.19</t>
+  </si>
+  <si>
+    <t>{'name': '$K_{n}^{r}$', 'definition': 'The complete $r$-uniform hypergraph on $n$ vertices.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'tightly connected', 'definition': 'In a $k$-uniform hypergraph $H$, $H$ is tightly connected if for every pair $u,v \\in V(H)$ there exist edges $e_{1},\\ldots,e_{p} \\in E(H)$ with $u \\in e_{1}$, $v \\in e_{p}$ and $|e_{i} \\cap e_{i+1}|=k-1$ for all $i$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$V(K)$', 'definition': 'The vertex set of $K$.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 4.3</t>
+  </si>
+  <si>
+    <t>{'name': '$\\alpha$', 'definition': '$\\alpha \\geq 1$ is an integer parameter; $\\alpha(G)$ is the independence number of $G$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$\\delta$', 'definition': 'A diameter bound depending on $\\alpha$, denoted $\\delta=\\delta(\\alpha)$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '\\mathrm{dc}_{r}^{\\delta}(G)', 'definition': 'The smallest integer $t$ such that in every $r$-coloring of the edges of $G$, there exists a monochromatic $t$-cover consisting of subgraphs of diameter at most $\\delta$.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 4.17</t>
+  </si>
+  <si>
+    <t>{'name': '$G$', 'definition': 'A complete graph whose edges are colored with 3 colors.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'monochromatic 2-cover', 'definition': 'A monochromatic cover of order at most $2$.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'diameter bound', 'definition': 'Each subgraph in the cover has $\\operatorname{diam} \\le 3$.'}</t>
+  </si>
+  <si>
+    <t>23-Conjecture 4.22</t>
+  </si>
+  <si>
+    <t>{'name': '$G$', 'definition': 'A complete 4-partite graph with partition $\\{V_{1},V_{2},V_{3},V_{4}\\}$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '[$V_{i},V_{j}$]', 'definition': 'The complete bipartite subgraph induced by the parts $V_{i}$ and $V_{j}$.'}</t>
+  </si>
+  <si>
+    <t>{'name': '$[5] \\backslash \\{i,j\\}$', 'definition': 'The set of colors used on $[V_{i},V_{j}]$ excludes the indices $i$ and $j$.'}</t>
+  </si>
+  <si>
+    <t>{'name': 'bounded diameter', 'definition': 'There exists an absolute constant $d$ such that each subgraph in the cover has $\\operatorname{diam} \\le d$.'}</t>
   </si>
 </sst>
 </file>
@@ -477,7 +660,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -908,10 +1091,10 @@
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -919,28 +1102,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -948,25 +1131,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -974,25 +1157,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1000,25 +1183,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1026,25 +1209,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1052,25 +1235,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1078,25 +1261,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1104,25 +1287,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1130,28 +1313,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1159,25 +1342,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1185,28 +1368,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1214,25 +1397,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1240,25 +1423,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
       </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1266,25 +1449,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1292,25 +1475,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1318,25 +1501,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H20" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1344,25 +1527,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1370,25 +1553,25 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1396,25 +1579,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H23" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1422,22 +1605,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" t="s">
-        <v>133</v>
-      </c>
-      <c r="E24" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>131</v>
+      <c r="H24" t="s">
+        <v>119</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>130</v>
@@ -1445,18 +1631,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G24" r:id="rId1" xr:uid="{98879843-8D25-4023-89BD-BA4BA592BD25}"/>
+    <hyperlink ref="G24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1469,13 +1655,189 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1485,22 +1847,448 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="231.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>175</v>
+      </c>
+      <c r="B34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
branchement du LLM au programme principal
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\Desktop\memoire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41FF15B-590C-482F-9847-333F1A0EC5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CF8C0A-ED98-444E-ADE0-157C0D152D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29280" yWindow="705" windowWidth="27255" windowHeight="13635" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="138">
   <si>
     <t>Id</t>
   </si>
@@ -423,54 +423,6 @@
     <t>Conjecture</t>
   </si>
   <si>
-    <t>These results suggest that NeuroSAT searches for a certificate of satisfiability, and that it only guesses sat once it has found one.</t>
-  </si>
-  <si>
-    <t>This suggests that NeuroSAT has not simply found a way to approximate SP, but rather has synthesized a qualitatively different algorithm.</t>
-  </si>
-  <si>
-    <t>Upon inspection, it seems to do so by learning to recognize the unsat cores.</t>
-  </si>
-  <si>
-    <t>We believe that their network's success is an instance of the phenomenon we study in this paper, namely that MPNNs can synthesize local search algorithms for constraint satisfaction problems.</t>
-  </si>
-  <si>
-    <t>We believe that architectures descended from NeuroSAT will be able to learn very different mechanisms and heuristics depending on the data they are trained on and the details of their objective functions.</t>
-  </si>
-  <si>
-    <t>We are cautiously optimistic that a descendant of NeuroSAT will one day lead to improvements to the state-of-the-art.</t>
-  </si>
-  <si>
-    <t>Conjecture 2.1. For all integers $r \geq 2$, all $S \subseteq[r]$, and all $r$-colorings of a complete graph $K$, there exists a monochromatic $(r-1)$-cover consisting entirely of subgraphs having a color in $S$ or consisting entirely of subgraphs having a color in $[r] \backslash S$.</t>
-  </si>
-  <si>
-    <t>Conjecture 2.2. For all integers $r \geq 2$ and all $K \in \mathcal{K}_{r}, \operatorname{tc}_{r-1}(K) \leq r-1$. In particular, this implies that for every $r$-coloring of a complete graph $K$ and every color $i \in[r]$, either there is a monochromatic $(r-1)$-cover consisting entirely of subgraphs of color $i$, or entirely of subgraphs which don't have color $i$.</t>
-  </si>
-  <si>
-    <t>Conjecture 2.3. For all integers $r \geq 3$ and all $K \in \mathcal{K}_{r-1}, \operatorname{tc}_{r-1}(K) \leq r-1$. In particular, this implies that for every $r$-coloring of a complete graph $K$ and every color $i \in[r]$, either there is a monochromatic $(r-2)$-cover consisting entirely of subgraphs of color $i$, or a monochromatic $(r-1)$-cover consisting entirely of subgraphs which don't have color $i$.</t>
-  </si>
-  <si>
-    <t>Conjecture 2.4. For all integers $r \geq 2$, in every $r$-coloring of a complete graph $K$ there exists a monochromatic $(r-1)$-cover such that the monochromatic subgraphs have at most $\lceil r / 2\rceil$ different colors.</t>
-  </si>
-  <si>
-    <t>Conjecture 2.8. For all $\alpha \geq 1$, there exists $d=d(\alpha)$ such that for all $r \geq 2$, if $G$ is a graph with $\alpha(G)=\alpha$, then in every $r$-coloring of $G$, there exists a monochromatic $(r-1) \alpha$-cover consisting of subgraphs of diameter at most $d$.</t>
-  </si>
-  <si>
-    <t>Conjecture 2.14. There exists $d$ such that for all $r \geq 2$, if $K \in \mathcal{K}_{2}$, then in every $r$-coloring of $K$, there exists a monochromatic $(2 r-2)$-cover consisting of subgraphs of diameter at most d.</t>
-  </si>
-  <si>
-    <t>Conjecture 2.19. For all $r \geq 3$, in every $r$-coloring of $K_{n}^{r}$, there exists a monochromatic tightly connected subgraph which covers $V(K)$.</t>
-  </si>
-  <si>
-    <t>Conjecture 4.3. For all $\alpha \geq 1$, there exists $\delta=\delta(\alpha)$ such that for all $r \geq 2$, if $G$ is a graph with $\alpha(G)=\alpha$, then $\mathrm{dc}_{r}^{\delta}(G) \leq(r-1) \alpha$.</t>
-  </si>
-  <si>
-    <t>Conjecture 4.17. Let $G$ be a 3-colored complete graph. There exists a monochromatic 2-cover consisting of subgraphs of diameter at most 3.</t>
-  </si>
-  <si>
-    <t>Conjecture 4.22. Suppose $G$ is a complete 4-partite graph with vertex set partitioned as $\left\{V_{1}, V_{2}, V_{3}, V_{4}\right\}$. If $\left[V_{i}, V_{j}\right]$ is colored with colors from $[5] \backslash\{i, j\}$ for all distinct $i, j \in[4]$, then $G$ can be covered with at most three monochromatic subgraphs of bounded diameter.</t>
-  </si>
-  <si>
     <t>Conjecture_id</t>
   </si>
   <si>
@@ -480,133 +432,10 @@
     <t>23-Conjecture 2.1</t>
   </si>
   <si>
-    <t>{'name': '$r$', 'definition': '$r$ is an integer with $r \\geq 2$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$S$', 'definition': '$S \\subseteq [r]$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$[r]$', 'definition': '$[r]=\\{1,2,\\dots,r\\}$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$K$', 'definition': '$K$ is a complete graph.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'r-coloring', 'definition': 'An $r$-coloring of the edges of a graph $G$ is a function $c:E(G) \\to [r]$; equivalently, a partition of $E(G)$ into (possibly empty) sets $\\{E_{1},\\ldots,E_{r}\\}$.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'monochromatic cover', 'definition': 'In an $r$-colored graph $H$, a monochromatic cover is a set $\\mathcal{T}$ of monochromatic connected subgraphs with $V(H)=\\cup_{T \\in \\mathcal{T}} V(T)$.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'monochromatic $t$-cover', 'definition': 'A monochromatic cover of order at most $t$.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 2.2</t>
-  </si>
-  <si>
-    <t>{'name': '$K$', 'definition': '$K \\in \\mathcal{K}_{r}$ is a complete $r$-partite graph.'}</t>
-  </si>
-  <si>
-    <t>{'name': '\\mathcal{K}_{k}', 'definition': 'For $k \\geq 2$, $\\mathcal{K}_{k}$ is the family of all complete $k$-partite graphs.'}</t>
-  </si>
-  <si>
-    <t>{'name': '\\operatorname{tc}_{r}(H)', 'definition': 'The minimum integer $t$ such that in every $r$-coloring of the edges of $H$, there exists a monochromatic $t$-cover of $H$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$i$', 'definition': '$i \\in [r]$ is a color index.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 2.3</t>
-  </si>
-  <si>
-    <t>{'name': '$r$', 'definition': '$r$ is an integer with $r \\geq 3$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$K$', 'definition': '$K \\in \\mathcal{K}_{r-1}$ is a complete $(r-1)$-partite graph.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 2.4</t>
-  </si>
-  <si>
-    <t>{'name': '\\lceil r/2 \\rceil', 'definition': 'The ceiling of $r/2$.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 2.8</t>
-  </si>
-  <si>
-    <t>{'name': '$\\alpha$', 'definition': '$\\alpha \\geq 1$ is an integer parameter.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$d$', 'definition': '$d=d(\\alpha)$ is a diameter bound depending on $\\alpha$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$G$', 'definition': '$G$ is a graph with $\\alpha(G)=\\alpha$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '\\alpha(G)', 'definition': 'The size of a maximum independent set of vertices in $G$.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'diameter', 'definition': 'For vertices $u,v \\in V(G)$, $d(u,v)$ is the length of the shortest $u,v$-path (or $\\infty$ if none exists); $\\operatorname{diam}(G)$ is the smallest $d$ with $d(u,v) \\le d$ for all $u,v \\in V(G)$.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 2.14</t>
-  </si>
-  <si>
-    <t>{'name': '$d$', 'definition': 'An absolute diameter bound.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$K$', 'definition': '$K \\in \\mathcal{K}_{2}$ is a complete bipartite graph.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 2.19</t>
-  </si>
-  <si>
-    <t>{'name': '$K_{n}^{r}$', 'definition': 'The complete $r$-uniform hypergraph on $n$ vertices.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'tightly connected', 'definition': 'In a $k$-uniform hypergraph $H$, $H$ is tightly connected if for every pair $u,v \\in V(H)$ there exist edges $e_{1},\\ldots,e_{p} \\in E(H)$ with $u \\in e_{1}$, $v \\in e_{p}$ and $|e_{i} \\cap e_{i+1}|=k-1$ for all $i$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$V(K)$', 'definition': 'The vertex set of $K$.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 4.3</t>
-  </si>
-  <si>
-    <t>{'name': '$\\alpha$', 'definition': '$\\alpha \\geq 1$ is an integer parameter; $\\alpha(G)$ is the independence number of $G$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$\\delta$', 'definition': 'A diameter bound depending on $\\alpha$, denoted $\\delta=\\delta(\\alpha)$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '\\mathrm{dc}_{r}^{\\delta}(G)', 'definition': 'The smallest integer $t$ such that in every $r$-coloring of the edges of $G$, there exists a monochromatic $t$-cover consisting of subgraphs of diameter at most $\\delta$.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 4.17</t>
-  </si>
-  <si>
-    <t>{'name': '$G$', 'definition': 'A complete graph whose edges are colored with 3 colors.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'monochromatic 2-cover', 'definition': 'A monochromatic cover of order at most $2$.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'diameter bound', 'definition': 'Each subgraph in the cover has $\\operatorname{diam} \\le 3$.'}</t>
-  </si>
-  <si>
-    <t>23-Conjecture 4.22</t>
-  </si>
-  <si>
-    <t>{'name': '$G$', 'definition': 'A complete 4-partite graph with partition $\\{V_{1},V_{2},V_{3},V_{4}\\}$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '[$V_{i},V_{j}$]', 'definition': 'The complete bipartite subgraph induced by the parts $V_{i}$ and $V_{j}$.'}</t>
-  </si>
-  <si>
-    <t>{'name': '$[5] \\backslash \\{i,j\\}$', 'definition': 'The set of colors used on $[V_{i},V_{j}]$ excludes the indices $i$ and $j$.'}</t>
-  </si>
-  <si>
-    <t>{'name': 'bounded diameter', 'definition': 'There exists an absolute constant $d$ such that each subgraph in the cover has $\\operatorname{diam} \\le d$.'}</t>
+    <t>Let G be a connected graph with x = radius and y = density, then y(G) &lt;= 4454599/6707305 + 496633/800000 * x(G) - 1145396/3571471 * x(G)^2 + 66746/1865747 * x(G)^2</t>
+  </si>
+  <si>
+    <t>Let G be a connected graph with x = radius and y = density, then y(G) &lt;= 4454599/6707305 + 496633/800000 * x(G) - 1145396/3571471 * x(G)^2 + 66746/1865747 * x(G)^3</t>
   </si>
 </sst>
 </file>
@@ -1640,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1669,175 +1498,10 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>145</v>
-      </c>
-      <c r="C14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1847,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1861,434 +1525,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>164</v>
-      </c>
-      <c r="B16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>164</v>
-      </c>
-      <c r="B18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>167</v>
-      </c>
-      <c r="B21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>167</v>
-      </c>
-      <c r="B23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>167</v>
-      </c>
-      <c r="B24" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>167</v>
-      </c>
-      <c r="B25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>169</v>
-      </c>
-      <c r="B26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>169</v>
-      </c>
-      <c r="B28" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>169</v>
-      </c>
-      <c r="B29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>169</v>
-      </c>
-      <c r="B30" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>169</v>
-      </c>
-      <c r="B31" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>169</v>
-      </c>
-      <c r="B32" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>175</v>
-      </c>
-      <c r="B34" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>175</v>
-      </c>
-      <c r="B35" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>175</v>
-      </c>
-      <c r="B36" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>175</v>
-      </c>
-      <c r="B37" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>175</v>
-      </c>
-      <c r="B38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>178</v>
-      </c>
-      <c r="B39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>178</v>
-      </c>
-      <c r="B40" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>178</v>
-      </c>
-      <c r="B41" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>178</v>
-      </c>
-      <c r="B42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>182</v>
-      </c>
-      <c r="B43" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>182</v>
-      </c>
-      <c r="B44" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>182</v>
-      </c>
-      <c r="B45" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>182</v>
-      </c>
-      <c r="B46" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B47" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
-        <v>186</v>
-      </c>
-      <c r="B48" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>186</v>
-      </c>
-      <c r="B50" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>190</v>
-      </c>
-      <c r="B51" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>190</v>
-      </c>
-      <c r="B52" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>190</v>
-      </c>
-      <c r="B53" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>190</v>
-      </c>
-      <c r="B54" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>